<commit_message>
Major Update: Enhanced Model Architecture, Documentation, and Performance Analysis
</commit_message>
<xml_diff>
--- a/arcticle/baseline.xlsx
+++ b/arcticle/baseline.xlsx
@@ -16,22 +16,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>method</t>
-  </si>
-  <si>
-    <t>accuracy</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>publication</t>
-  </si>
-  <si>
-    <t>ours</t>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Publication</t>
+  </si>
+  <si>
+    <t>Our Method</t>
   </si>
   <si>
     <t>HyGPR-Net</t>
@@ -78,10 +78,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -109,20 +109,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -151,10 +137,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -174,40 +161,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,6 +184,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -230,15 +238,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,19 +253,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,163 +415,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -473,20 +473,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,15 +510,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -530,17 +525,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -550,10 +550,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -562,133 +562,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1023,8 +1023,8 @@
   <sheetPr/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.85" outlineLevelRow="6" outlineLevelCol="4"/>

</xml_diff>